<commit_message>
committing date picker change and database updates
</commit_message>
<xml_diff>
--- a/csimcw_db_schema.xlsx
+++ b/csimcw_db_schema.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="15180" windowHeight="4755"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="15180" windowHeight="4755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Database Details" sheetId="1" r:id="rId1"/>
     <sheet name="Features" sheetId="2" r:id="rId2"/>
     <sheet name="Task List" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="144">
   <si>
     <t>Database Design</t>
   </si>
@@ -171,12 +171,6 @@
     <t>SL.No</t>
   </si>
   <si>
-    <t>Family</t>
-  </si>
-  <si>
-    <t>fly_id</t>
-  </si>
-  <si>
     <t>member_id</t>
   </si>
   <si>
@@ -189,9 +183,6 @@
     <t>boolean</t>
   </si>
   <si>
-    <t>image</t>
-  </si>
-  <si>
     <t>Subscriptions</t>
   </si>
   <si>
@@ -442,6 +433,21 @@
   </si>
   <si>
     <t>in progress</t>
+  </si>
+  <si>
+    <t>Member Details</t>
+  </si>
+  <si>
+    <t>individual_id</t>
+  </si>
+  <si>
+    <t>image_path</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>last_modified_date</t>
   </si>
 </sst>
 </file>
@@ -1031,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1316,7 +1322,7 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E19" s="2">
         <v>15</v>
@@ -1332,7 +1338,7 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E20" s="2">
         <v>15</v>
@@ -1348,7 +1354,7 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E21" s="2">
         <v>15</v>
@@ -1364,7 +1370,7 @@
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E22" s="2">
         <v>15</v>
@@ -1585,7 +1591,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="31" t="s">
-        <v>51</v>
+        <v>139</v>
       </c>
       <c r="B38" s="32"/>
       <c r="C38" s="32"/>
@@ -1618,7 +1624,7 @@
         <v>1</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>52</v>
+        <v>140</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
@@ -1628,7 +1634,7 @@
         <v>11</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1636,7 +1642,7 @@
         <v>2</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
@@ -1646,7 +1652,7 @@
         <v>11</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1654,7 +1660,7 @@
         <v>3</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
@@ -1704,7 +1710,7 @@
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="3"/>
@@ -1718,7 +1724,7 @@
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="3"/>
@@ -1732,7 +1738,7 @@
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="3"/>
@@ -1756,7 +1762,7 @@
         <v>10</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>57</v>
+        <v>141</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
@@ -1776,62 +1782,80 @@
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="3"/>
     </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="5">
+        <v>12</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="5">
+        <v>13</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="3"/>
+    </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="B53" s="32"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="33"/>
+      <c r="A53" s="28"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="17"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="33"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B55" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C55" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D54" s="9" t="s">
+      <c r="D55" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E54" s="9" t="s">
+      <c r="E55" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F54" s="9" t="s">
+      <c r="F55" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="30">
-      <c r="A55" s="2">
+    <row r="56" spans="1:6" ht="30">
+      <c r="A56" s="2">
         <v>1</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E55" s="2">
-        <v>11</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="2">
-        <v>2</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>59</v>
@@ -1843,14 +1867,16 @@
       <c r="E56" s="2">
         <v>11</v>
       </c>
-      <c r="F56" s="3"/>
+      <c r="F56" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2" t="s">
@@ -1859,144 +1885,142 @@
       <c r="E57" s="2">
         <v>11</v>
       </c>
-      <c r="F57" s="2"/>
+      <c r="F57" s="3"/>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E58" s="2">
-        <v>255</v>
+        <v>11</v>
       </c>
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E59" s="2">
-        <v>25</v>
+        <v>255</v>
       </c>
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>69</v>
+        <v>11</v>
+      </c>
+      <c r="E60" s="2">
+        <v>25</v>
       </c>
       <c r="F60" s="2"/>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="E61" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" s="2">
-        <v>100</v>
       </c>
       <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2">
+        <v>7</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="2">
+        <v>100</v>
+      </c>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="2">
         <v>8</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E62" s="2">
+      <c r="C63" s="2"/>
+      <c r="D63" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E63" s="2">
         <v>1</v>
       </c>
-      <c r="F62" s="2"/>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="B64" s="32"/>
-      <c r="C64" s="32"/>
-      <c r="D64" s="32"/>
-      <c r="E64" s="32"/>
-      <c r="F64" s="33"/>
+      <c r="F63" s="2"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="9" t="s">
+      <c r="A65" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65" s="32"/>
+      <c r="C65" s="32"/>
+      <c r="D65" s="32"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="33"/>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B66" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C66" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="9" t="s">
+      <c r="D66" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E65" s="9" t="s">
+      <c r="E66" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="9" t="s">
+      <c r="F66" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="30">
-      <c r="A66" s="2">
+    <row r="67" spans="1:6" ht="30">
+      <c r="A67" s="2">
         <v>1</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E66" s="2">
-        <v>11</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="2">
-        <v>2</v>
-      </c>
       <c r="B67" s="2" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
@@ -2005,14 +2029,16 @@
       <c r="E67" s="2">
         <v>11</v>
       </c>
-      <c r="F67" s="3"/>
+      <c r="F67" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
@@ -2021,81 +2047,97 @@
       <c r="E68" s="2">
         <v>11</v>
       </c>
-      <c r="F68" s="2"/>
+      <c r="F68" s="3"/>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E69" s="2">
+        <v>11</v>
+      </c>
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="2">
+        <v>4</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="2">
         <v>255</v>
       </c>
-      <c r="F69" s="2"/>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="5">
-        <v>5</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C70" s="2"/>
-      <c r="D70" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" s="5">
-        <v>255</v>
-      </c>
-      <c r="F70" s="3"/>
+      <c r="F70" s="2"/>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>77</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C71" s="2"/>
       <c r="D71" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E71" s="5">
-        <v>10</v>
+        <v>255</v>
       </c>
       <c r="F71" s="3"/>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="5">
+        <v>6</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" s="5">
+        <v>10</v>
+      </c>
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="5">
         <v>7</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C72" s="2"/>
-      <c r="D72" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E72" s="5">
+      <c r="B73" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C73" s="2"/>
+      <c r="D73" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E73" s="5">
         <v>15</v>
       </c>
-      <c r="F72" s="3"/>
+      <c r="F73" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A64:F64"/>
-    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="A54:F54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2105,7 +2147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -2117,17 +2159,17 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="35" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>3</v>
@@ -2138,10 +2180,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30">
@@ -2149,10 +2191,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30">
@@ -2160,10 +2202,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45">
@@ -2171,10 +2213,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30">
@@ -2182,10 +2224,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30">
@@ -2193,10 +2235,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45">
@@ -2204,10 +2246,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30">
@@ -2215,10 +2257,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="45">
@@ -2226,10 +2268,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30">
@@ -2237,10 +2279,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30">
@@ -2248,10 +2290,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30">
@@ -2259,10 +2301,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2277,8 +2319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:L22"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2294,34 +2336,34 @@
   <sheetData>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" s="24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I3" s="25" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30">
@@ -2329,10 +2371,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D4" s="12">
         <v>1</v>
@@ -2341,15 +2383,15 @@
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
       <c r="H4" s="29" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="14"/>
       <c r="K4" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30">
@@ -2357,10 +2399,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D5" s="16">
         <v>2</v>
@@ -2369,7 +2411,7 @@
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
       <c r="H5" s="29" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I5" s="16"/>
       <c r="J5" s="18"/>
@@ -2379,10 +2421,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D6" s="16">
         <v>4</v>
@@ -2391,7 +2433,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="18"/>
@@ -2401,10 +2443,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D7" s="16">
         <v>4</v>
@@ -2413,7 +2455,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="30" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I7" s="16"/>
       <c r="J7" s="18"/>
@@ -2423,10 +2465,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>122</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>125</v>
       </c>
       <c r="D8" s="16">
         <v>5</v>
@@ -2435,7 +2477,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I8" s="16"/>
       <c r="J8" s="18"/>
@@ -2445,10 +2487,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D9" s="16">
         <v>4</v>
@@ -2457,7 +2499,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I9" s="16"/>
       <c r="J9" s="18"/>
@@ -2467,10 +2509,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D10" s="16">
         <v>2</v>
@@ -2479,7 +2521,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="18"/>
@@ -2489,10 +2531,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D11" s="16">
         <v>4</v>
@@ -2501,7 +2543,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="18"/>
@@ -2511,17 +2553,17 @@
         <v>9</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I12" s="16"/>
       <c r="J12" s="18"/>
@@ -2531,17 +2573,17 @@
         <v>10</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="H13" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I13" s="16"/>
       <c r="J13" s="18"/>
@@ -2551,17 +2593,17 @@
         <v>11</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
       <c r="H14" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I14" s="16"/>
       <c r="J14" s="18"/>
@@ -2571,17 +2613,17 @@
         <v>12</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
       <c r="H15" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I15" s="16"/>
       <c r="J15" s="18"/>
@@ -2591,17 +2633,17 @@
         <v>13</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
       <c r="H16" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I16" s="16"/>
       <c r="J16" s="18"/>
@@ -2611,17 +2653,17 @@
         <v>14</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
       <c r="H17" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I17" s="16"/>
       <c r="J17" s="18"/>
@@ -2631,7 +2673,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="16"/>
@@ -2639,7 +2681,7 @@
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
       <c r="H18" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I18" s="16"/>
       <c r="J18" s="18"/>
@@ -2649,7 +2691,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="16"/>
@@ -2657,7 +2699,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
       <c r="H19" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I19" s="16"/>
       <c r="J19" s="18"/>

</xml_diff>